<commit_message>
finalized data and completed script for main.js
</commit_message>
<xml_diff>
--- a/chapter1/data/spatiotempdata.xlsx
+++ b/chapter1/data/spatiotempdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medst\Dropbox\Grad School\Fall 2023\Geog575\unit-1-master\unit-2\chapter1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medst\Dropbox\Grad School\Fall 2023\Geog575\unit-2\unit-2\chapter1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0809FD4-E1C5-4C8F-8F3F-0B6E6C820DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D990F672-C320-4000-A845-31A8EF9F1074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{9F1ACF37-6E63-439C-AC7F-05EEE91F7D92}"/>
   </bookViews>
@@ -36,36 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>featName</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>lon</t>
-  </si>
-  <si>
-    <t>elevation</t>
-  </si>
-  <si>
-    <t>annualTempMax</t>
-  </si>
-  <si>
-    <t>annualTempMin</t>
-  </si>
-  <si>
-    <t>stationName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>uniqueID</t>
-  </si>
-  <si>
-    <t>annualPrecip</t>
-  </si>
-  <si>
-    <t>stationID</t>
   </si>
 </sst>
 </file>
@@ -417,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D9F1A1-D8D0-49D8-94FF-640C116205E9}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -430,36 +403,9 @@
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
         <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>